<commit_message>
Merged PR 12983: Integration Test Repair : ProgramMapping
Test Repair
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Program Mapping/ProgramMappingsMappedGenre.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Program Mapping/ProgramMappingsMappedGenre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bbotelho\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\Program Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sespiritu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0A7185D-EE61-46B3-97BE-A6489ACE6837}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7C5DAE-0BD4-4EA7-B411-F906824B2C58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{32575155-09DC-45E3-843C-2D66AF1A0F1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27375" windowHeight="16440" xr2:uid="{32575155-09DC-45E3-843C-2D66AF1A0F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Series</t>
   </si>
   <si>
-    <t>Action</t>
+    <t>Drama</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>